<commit_message>
ability to choose ouput excel rows
</commit_message>
<xml_diff>
--- a/Marijus_Mozdeikis/results/resonance_properties.xlsx
+++ b/Marijus_Mozdeikis/results/resonance_properties.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="20250722_05nJ_08um" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="All_Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,7 +523,7 @@
         <v>932.02</v>
       </c>
       <c r="E3" t="n">
-        <v>39.41238033783407</v>
+        <v>42.84628741893843</v>
       </c>
       <c r="F3" t="n">
         <v>12.05999999999995</v>
@@ -532,7 +532,7 @@
         <v>77.28192371475988</v>
       </c>
       <c r="H3" t="n">
-        <v>-30.45864570685595</v>
+        <v>-33.11243515771076</v>
       </c>
     </row>
     <row r="4">
@@ -583,7 +583,7 @@
         <v>1023.99</v>
       </c>
       <c r="E5" t="n">
-        <v>36.99164893607099</v>
+        <v>40.69499103768919</v>
       </c>
       <c r="F5" t="n">
         <v>11.94000000000005</v>
@@ -592,7 +592,7 @@
         <v>85.76130653266293</v>
       </c>
       <c r="H5" t="n">
-        <v>-31.72452143555039</v>
+        <v>-34.90055600727234</v>
       </c>
     </row>
     <row r="6">
@@ -643,7 +643,7 @@
         <v>1212.02</v>
       </c>
       <c r="E7" t="n">
-        <v>28.82444676498346</v>
+        <v>34.566222290819</v>
       </c>
       <c r="F7" t="n">
         <v>8.079999999999927</v>
@@ -652,7 +652,7 @@
         <v>150.0024752475261</v>
       </c>
       <c r="H7" t="n">
-        <v>-43.23738362388066</v>
+        <v>-51.85018903579062</v>
       </c>
     </row>
     <row r="8">
@@ -673,7 +673,7 @@
         <v>795.96</v>
       </c>
       <c r="E8" t="n">
-        <v>13.37017977742175</v>
+        <v>16.31675477022422</v>
       </c>
       <c r="F8" t="n">
         <v>27.96000000000004</v>
@@ -682,7 +682,7 @@
         <v>28.46781115879825</v>
       </c>
       <c r="H8" t="n">
-        <v>-3.806197530628257</v>
+        <v>-4.645022935231637</v>
       </c>
     </row>
     <row r="9">
@@ -703,16 +703,16 @@
         <v>1376.09</v>
       </c>
       <c r="E9" t="n">
-        <v>24.65624363694739</v>
+        <v>34.26292324808001</v>
       </c>
       <c r="F9" t="n">
-        <v>8.039999999999964</v>
+        <v>12.06999999999994</v>
       </c>
       <c r="G9" t="n">
-        <v>171.1554726368167</v>
+        <v>114.0091135045573</v>
       </c>
       <c r="H9" t="n">
-        <v>-42.20051033130235</v>
+        <v>-39.06285505588291</v>
       </c>
     </row>
     <row r="10">
@@ -733,7 +733,7 @@
         <v>799.96</v>
       </c>
       <c r="E10" t="n">
-        <v>14.57500817007217</v>
+        <v>17.59011398772621</v>
       </c>
       <c r="F10" t="n">
         <v>19.96000000000004</v>
@@ -742,7 +742,7 @@
         <v>40.07815631262518</v>
       </c>
       <c r="H10" t="n">
-        <v>-5.841394556979415</v>
+        <v>-7.049793379569858</v>
       </c>
     </row>
     <row r="11">
@@ -763,16 +763,16 @@
         <v>1499.99</v>
       </c>
       <c r="E11" t="n">
-        <v>22.19138397138545</v>
+        <v>29.33483889098937</v>
       </c>
       <c r="F11" t="n">
-        <v>7.980000000000018</v>
+        <v>40.04999999999995</v>
       </c>
       <c r="G11" t="n">
-        <v>187.9686716791976</v>
+        <v>37.45293383270916</v>
       </c>
       <c r="H11" t="n">
-        <v>-41.71284967824359</v>
+        <v>-10.98675779977408</v>
       </c>
     </row>
     <row r="12">
@@ -793,7 +793,7 @@
         <v>804.05</v>
       </c>
       <c r="E12" t="n">
-        <v>31.40909479619052</v>
+        <v>34.23011461117398</v>
       </c>
       <c r="F12" t="n">
         <v>12.09999999999991</v>
@@ -802,7 +802,7 @@
         <v>66.450413223141</v>
       </c>
       <c r="H12" t="n">
-        <v>-20.87147328171667</v>
+        <v>-22.74605260587987</v>
       </c>
     </row>
     <row r="13">
@@ -823,7 +823,7 @@
         <v>788.02</v>
       </c>
       <c r="E13" t="n">
-        <v>31.44248528981313</v>
+        <v>32.98968159783203</v>
       </c>
       <c r="F13" t="n">
         <v>16.00999999999999</v>
@@ -832,7 +832,7 @@
         <v>49.22048719550284</v>
       </c>
       <c r="H13" t="n">
-        <v>-15.47614444602034</v>
+        <v>-16.23768200669807</v>
       </c>
     </row>
     <row r="14">
@@ -922,6 +922,66 @@
         <v>17.88837209302323</v>
       </c>
       <c r="H16" t="n">
+        <v>-5.248851284020017</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>20250722_05nJ_08um.xlsx</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.8um, R 45 S </t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>603.99</v>
+      </c>
+      <c r="E17" t="n">
+        <v>32.95886841854031</v>
+      </c>
+      <c r="F17" t="n">
+        <v>19.96000000000004</v>
+      </c>
+      <c r="G17" t="n">
+        <v>30.26002004008011</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-9.973360188433931</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>20250722_05nJ_08um.xlsx</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.8um, R 60 S </t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>499.98</v>
+      </c>
+      <c r="E18" t="n">
+        <v>29.34225236776665</v>
+      </c>
+      <c r="F18" t="n">
+        <v>27.95000000000005</v>
+      </c>
+      <c r="G18" t="n">
+        <v>17.88837209302323</v>
+      </c>
+      <c r="H18" t="n">
         <v>-5.248851284020017</v>
       </c>
     </row>

</xml_diff>